<commit_message>
update question set for my girlfriend
</commit_message>
<xml_diff>
--- a/create-questions/questions.xlsx
+++ b/create-questions/questions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\svelte-quiz\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\svelte-quiz\create-questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA9281B-27AB-49DD-AE24-22FFD1E9E102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30CF8331-3382-4B37-AC8F-C26235817823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9449F812-5DC8-46AF-9392-C264B1A25776}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="167">
   <si>
     <t>type</t>
   </si>
@@ -402,6 +402,141 @@
   </si>
   <si>
     <t>Cá nhân | Chính trị - pháp luật | Công nghệ</t>
+  </si>
+  <si>
+    <t>Kế hoạch hưu trí giúp bạn đạt được điều gì?</t>
+  </si>
+  <si>
+    <t>An toàn và độc lập tài chính khi nghỉ hưu</t>
+  </si>
+  <si>
+    <t>Mua bảo hiểm nhân thọ với lãi suất cao | Tăng thu nhập ngay lập tức | Đầu tư bất động sản</t>
+  </si>
+  <si>
+    <t>Mục tiêu của việc lập kế hoạch hưu trí là gì?</t>
+  </si>
+  <si>
+    <t>Đảm bảo cuộc sống ổn định và thoải mái sau khi nghỉ hưu</t>
+  </si>
+  <si>
+    <t>Đảm bảo chi phí học tập cho con cái | Đầu tư vào thị trường chứng khoán | Chỉ bảo vệ tài sản</t>
+  </si>
+  <si>
+    <t>Lợi ích nào sau đây KHÔNG phải của kế hoạch hưu trí?</t>
+  </si>
+  <si>
+    <t>Tạo ra nhiều khoản vay dài hạn</t>
+  </si>
+  <si>
+    <t>Độc lập tài chính | An toàn tài chính | Dự phòng rủi ro</t>
+  </si>
+  <si>
+    <t>Một trong những vai trò chính của kế hoạch hưu trí là gì?</t>
+  </si>
+  <si>
+    <t>Giúp bạn quản lý tài chính dài hạn hiệu quả</t>
+  </si>
+  <si>
+    <t>Giúp bạn vay vốn với lãi suất thấp | Đảm bảo giá trị bất động sản | Giảm chi phí sinh hoạt hàng ngày</t>
+  </si>
+  <si>
+    <t>Tại sao nên tối ưu hóa thuế trong kế hoạch hưu trí?</t>
+  </si>
+  <si>
+    <t>Giúp bạn tận dụng các lợi ích thuế từ các khoản đầu tư hưu trí</t>
+  </si>
+  <si>
+    <t>Để có thêm nhiều khoản nợ mới | Để tăng số lượng tài sản nắm giữ | Để giảm số năm làm việc</t>
+  </si>
+  <si>
+    <t>Quy trình lập kế hoạch hưu trí bắt đầu với bước nào?</t>
+  </si>
+  <si>
+    <t>Xác định mục tiêu hưu trí</t>
+  </si>
+  <si>
+    <t>Đầu tư vào chứng khoán | Giảm chi tiêu hàng ngày | Vay vốn từ ngân hàng</t>
+  </si>
+  <si>
+    <t>Khi xác định mục tiêu hưu trí, cần xem xét yếu tố nào?</t>
+  </si>
+  <si>
+    <t>Tuổi nghỉ hưu và mức sống mong muốn</t>
+  </si>
+  <si>
+    <t>Chỉ tiêu tài chính của công ty | Các khoản nợ cá nhân | Mức thu nhập tối đa hiện tại</t>
+  </si>
+  <si>
+    <t>Đánh giá tài chính hiện tại bao gồm những gì?</t>
+  </si>
+  <si>
+    <t>Tài sản, nợ, thu nhập, và chi tiêu</t>
+  </si>
+  <si>
+    <t>Chỉ gồm lương hưu | Các khoản nợ ngắn hạn | Số tiền vay dự kiến</t>
+  </si>
+  <si>
+    <t>Để ước tính chi phí hưu trí, cần xem xét chi phí nào?</t>
+  </si>
+  <si>
+    <t>Chi phí sinh hoạt và chi phí y tế</t>
+  </si>
+  <si>
+    <t>Chi phí mua sắm hàng ngày | Chi phí kinh doanh | Chi phí học tập của con cái</t>
+  </si>
+  <si>
+    <t>Một phương pháp phổ biến để tính tổng chi phí cho giai đoạn nghỉ hưu là gì?</t>
+  </si>
+  <si>
+    <t>Nhân tổng chi phí hàng năm với số năm dự kiến sống sau khi nghỉ hưu</t>
+  </si>
+  <si>
+    <t>Chia tổng chi phí cho 12 tháng | Nhân tổng thu nhập với lãi suất | Trừ tổng chi phí hàng năm cho số năm làm việc</t>
+  </si>
+  <si>
+    <t>Đặt mục tiêu tiết kiệm hàng tháng</t>
+  </si>
+  <si>
+    <t>Vay ngân hàng với lãi suất cao | Chỉ đầu tư vào bất động sản | Cắt giảm chi phí đầu tư</t>
+  </si>
+  <si>
+    <t>Để đạt được số tiền hưu trí cần thiết, nên làm gì?</t>
+  </si>
+  <si>
+    <t>Khi lập kế hoạch đầu tư cho hưu trí, cần cân nhắc yếu tố nào?</t>
+  </si>
+  <si>
+    <t>Khả năng chấp nhận rủi ro</t>
+  </si>
+  <si>
+    <t>hỉ đầu tư vào tài sản có giá trị cao | Bỏ qua lợi nhuận dự kiến | Không quan tâm đến rủi ro</t>
+  </si>
+  <si>
+    <t>Các nguồn thu nhập hưu trí bao gồm gì?</t>
+  </si>
+  <si>
+    <t>Quỹ hưu trí và lợi nhuận từ đầu tư</t>
+  </si>
+  <si>
+    <t>Khoản vay ngắn hạn | Thu nhập từ việc làm thêm | Bán tài sản hằng năm</t>
+  </si>
+  <si>
+    <t>Khi nào cần đánh giá lại kế hoạch hưu trí?</t>
+  </si>
+  <si>
+    <t>Định kỳ hoặc khi có thay đổi trong tình hình tài chính</t>
+  </si>
+  <si>
+    <t>Khi hết nguồn thu nhập | Khi giá trị tài sản tăng | Khi muốn đầu tư vào bất động sản</t>
+  </si>
+  <si>
+    <t>Vì sao cần điều chỉnh kế hoạch hưu trí?</t>
+  </si>
+  <si>
+    <t>Để đảm bảo kế hoạch phù hợp với tình hình tài chính hiện tại</t>
+  </si>
+  <si>
+    <t>Để giảm chi phí sinh hoạt sau này | Để giảm số năm dự kiến nghỉ hưu | Để tăng khoản nợ ngân hàng</t>
   </si>
 </sst>
 </file>
@@ -444,10 +579,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -783,781 +916,1080 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96BDBFF7-410E-4581-AA17-BB64B0E0BD7F}">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="35.77734375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="28.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.88671875" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="35.77734375" customWidth="1"/>
+    <col min="5" max="5" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" t="s">
         <v>55</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" t="s">
         <v>58</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="1" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>65</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" t="s">
         <v>67</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
         <v>120</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="1" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" t="s">
         <v>61</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" t="s">
         <v>63</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="1" t="s">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="2" t="s">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="2" t="s">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="2" t="s">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="2" t="s">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" t="s">
         <v>34</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" s="2" t="s">
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="2" t="s">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" t="s">
         <v>41</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" t="s">
         <v>44</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="2" t="s">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" t="s">
         <v>68</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" t="s">
         <v>69</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="2" t="s">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" t="s">
         <v>74</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" t="s">
         <v>39</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="2" t="s">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" t="s">
         <v>71</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" t="s">
         <v>72</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F20" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" s="2" t="s">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" t="s">
         <v>75</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" t="s">
         <v>76</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D22" s="2" t="s">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" t="s">
         <v>78</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" t="s">
         <v>79</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F22" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D23" s="2" t="s">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" t="s">
         <v>81</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" t="s">
         <v>82</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F23" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D24" s="2" t="s">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" t="s">
         <v>84</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" t="s">
         <v>85</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F24" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D25" s="2" t="s">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" t="s">
         <v>90</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" t="s">
         <v>91</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D26" s="2" t="s">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" t="s">
         <v>93</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" t="s">
         <v>94</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F26" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D27" s="2" t="s">
+      <c r="A27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" t="s">
         <v>96</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" t="s">
         <v>97</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="F27" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D28" s="2" t="s">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" t="s">
         <v>99</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" t="s">
         <v>100</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F28" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D29" s="2" t="s">
+      <c r="A29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" t="s">
         <v>102</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" t="s">
         <v>103</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="F29" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D30" s="2" t="s">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" t="s">
+        <v>42</v>
+      </c>
+      <c r="D30" t="s">
         <v>105</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" t="s">
         <v>106</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F30" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D31" s="2" t="s">
+      <c r="A31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31" t="s">
         <v>108</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" t="s">
         <v>109</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="F31" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D32" s="2" t="s">
+      <c r="A32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" t="s">
         <v>111</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" t="s">
         <v>112</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F32" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D33" s="2" t="s">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" t="s">
         <v>114</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E33" t="s">
         <v>115</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F33" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D34" s="1" t="s">
+      <c r="A34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34" t="s">
         <v>117</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E34" t="s">
         <v>118</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="F34" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D35" s="2" t="s">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" t="s">
+        <v>42</v>
+      </c>
+      <c r="D35" t="s">
         <v>87</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E35" t="s">
         <v>88</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="F35" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" s="1" t="s">
+      <c r="A36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" t="s">
         <v>45</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D36" t="s">
         <v>46</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E36" t="s">
         <v>47</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="F36" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" s="1" t="s">
+      <c r="A37" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" t="s">
         <v>45</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D37" t="s">
         <v>52</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E37" t="s">
         <v>53</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="F37" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" s="1" t="s">
+      <c r="A38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" t="s">
         <v>45</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D38" t="s">
         <v>49</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E38" t="s">
         <v>50</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="F38" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" t="s">
+        <v>45</v>
+      </c>
+      <c r="D39" t="s">
+        <v>122</v>
+      </c>
+      <c r="E39" t="s">
+        <v>123</v>
+      </c>
+      <c r="F39" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" t="s">
+        <v>45</v>
+      </c>
+      <c r="D40" t="s">
+        <v>125</v>
+      </c>
+      <c r="E40" t="s">
+        <v>126</v>
+      </c>
+      <c r="F40" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" t="s">
+        <v>45</v>
+      </c>
+      <c r="D41" t="s">
+        <v>128</v>
+      </c>
+      <c r="E41" t="s">
+        <v>129</v>
+      </c>
+      <c r="F41" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" t="s">
+        <v>45</v>
+      </c>
+      <c r="D42" t="s">
+        <v>131</v>
+      </c>
+      <c r="E42" t="s">
+        <v>132</v>
+      </c>
+      <c r="F42" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" t="s">
+        <v>45</v>
+      </c>
+      <c r="D43" t="s">
+        <v>134</v>
+      </c>
+      <c r="E43" t="s">
+        <v>135</v>
+      </c>
+      <c r="F43" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" t="s">
+        <v>45</v>
+      </c>
+      <c r="D44" t="s">
+        <v>137</v>
+      </c>
+      <c r="E44" t="s">
+        <v>138</v>
+      </c>
+      <c r="F44" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" t="s">
+        <v>45</v>
+      </c>
+      <c r="D45" t="s">
+        <v>140</v>
+      </c>
+      <c r="E45" t="s">
+        <v>141</v>
+      </c>
+      <c r="F45" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" t="s">
+        <v>45</v>
+      </c>
+      <c r="D46" t="s">
+        <v>143</v>
+      </c>
+      <c r="E46" t="s">
+        <v>144</v>
+      </c>
+      <c r="F46" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>4</v>
+      </c>
+      <c r="B47" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47" t="s">
+        <v>45</v>
+      </c>
+      <c r="D47" t="s">
+        <v>146</v>
+      </c>
+      <c r="E47" t="s">
+        <v>147</v>
+      </c>
+      <c r="F47" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" t="s">
+        <v>45</v>
+      </c>
+      <c r="D48" t="s">
+        <v>149</v>
+      </c>
+      <c r="E48" t="s">
+        <v>150</v>
+      </c>
+      <c r="F48" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49" t="s">
+        <v>45</v>
+      </c>
+      <c r="D49" t="s">
+        <v>154</v>
+      </c>
+      <c r="E49" t="s">
+        <v>152</v>
+      </c>
+      <c r="F49" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>4</v>
+      </c>
+      <c r="B50" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" t="s">
+        <v>45</v>
+      </c>
+      <c r="D50" t="s">
+        <v>155</v>
+      </c>
+      <c r="E50" t="s">
+        <v>156</v>
+      </c>
+      <c r="F50" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>4</v>
+      </c>
+      <c r="B51" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" t="s">
+        <v>45</v>
+      </c>
+      <c r="D51" t="s">
+        <v>158</v>
+      </c>
+      <c r="E51" t="s">
+        <v>159</v>
+      </c>
+      <c r="F51" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>4</v>
+      </c>
+      <c r="B52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" t="s">
+        <v>45</v>
+      </c>
+      <c r="D52" t="s">
+        <v>161</v>
+      </c>
+      <c r="E52" t="s">
+        <v>162</v>
+      </c>
+      <c r="F52" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>4</v>
+      </c>
+      <c r="B53" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" t="s">
+        <v>45</v>
+      </c>
+      <c r="D53" t="s">
+        <v>164</v>
+      </c>
+      <c r="E53" t="s">
+        <v>165</v>
+      </c>
+      <c r="F53" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>